<commit_message>
Spreadsheet import: added 'barcode' to Bin, Box columns
</commit_message>
<xml_diff>
--- a/public/CSV_Import.xlsx
+++ b/public/CSV_Import.xlsx
@@ -317,12 +317,6 @@
     <t>B-CSHM</t>
   </si>
   <si>
-    <t>Bin</t>
-  </si>
-  <si>
-    <t>Box</t>
-  </si>
-  <si>
     <t>Case Sensitivity</t>
   </si>
   <si>
@@ -354,7 +348,14 @@
     <t>A blank or 0 value will not attempt to assign a Box or Bin.  Entering an MDPI Barcode value will attempt to use existing Bin/Box if found, or create a new one if not found.  Entering an invalid barcode, or one already assigned to a Physical Object, will produce an error.  Note that it is preferable to create Bins beforehand, as the Identifier and Description values will be assigned unhelpful default values if created on-demand via spreadsheet upload.</t>
   </si>
   <si>
-    <t>Bin, Box</t>
+    <t>Bin barcode,
+Box barcode</t>
+  </si>
+  <si>
+    <t>Bin barcode</t>
+  </si>
+  <si>
+    <t>Box barcode</t>
   </si>
 </sst>
 </file>
@@ -507,9 +508,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -517,6 +515,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -943,58 +944,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="8" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="9" t="s">
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="10" t="s">
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
     </row>
     <row r="2" spans="1:37" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -1104,7 +1105,7 @@
     </row>
     <row r="3" spans="1:37" ht="63" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -1199,7 +1200,7 @@
     </row>
     <row r="4" spans="1:37" ht="63" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -1296,10 +1297,10 @@
     </row>
     <row r="2" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>50</v>
@@ -1313,13 +1314,13 @@
     </row>
     <row r="3" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1370,10 +1371,10 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1599,10 +1600,10 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -1832,10 +1833,10 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1921,7 +1922,7 @@
     </row>
     <row r="2" spans="1:29" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D2" s="4">
         <v>40000000000002</v>
@@ -2000,7 +2001,7 @@
     </row>
     <row r="3" spans="1:29" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D3" s="4">
         <v>40000000000010</v>

</xml_diff>

<commit_message>
Updated spreadsheet import with Bin identifier field
</commit_message>
<xml_diff>
--- a/public/CSV_Import.xlsx
+++ b/public/CSV_Import.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="104">
   <si>
     <t>Physical Object basic metadata fields</t>
   </si>
@@ -343,13 +343,6 @@
   </si>
   <si>
     <t>Bin/Box Assignment (by MDPI barcode)</t>
-  </si>
-  <si>
-    <t>A blank or 0 value will not attempt to assign a Box or Bin.  Entering an MDPI Barcode value will attempt to use existing Bin/Box if found, or create a new one if not found.  Entering an invalid barcode, or one already assigned to a Physical Object, will produce an error.  Note that it is preferable to create Bins beforehand, as the Identifier and Description values will be assigned unhelpful default values if created on-demand via spreadsheet upload.</t>
-  </si>
-  <si>
-    <t>Bin barcode,
-Box barcode</t>
   </si>
   <si>
     <t>Bin barcode</t>
@@ -417,6 +410,16 @@
       </rPr>
       <t>Leave blank for stand-alone items.  For grouped items: set to position value.</t>
     </r>
+  </si>
+  <si>
+    <t>Bin identifier</t>
+  </si>
+  <si>
+    <t>Bin barcode, Bin identifier,
+Box barcode</t>
+  </si>
+  <si>
+    <t>A blank or 0 value will not attempt to assign a Box or Bin.  Entering an MDPI Barcode value will attempt to use existing Bin/Box if found, or create a new one if not found.  Entering an invalid barcode, or one already assigned to a Physical Object, will produce an error.  Note creating a Bin via spreadsheet upload will generate a default Bin description.</t>
   </si>
 </sst>
 </file>
@@ -569,6 +572,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -580,9 +586,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="38">
@@ -960,392 +963,398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN4"/>
+  <dimension ref="A1:AO4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:V1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.875" style="1"/>
-    <col min="3" max="3" width="14.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="17.125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="7.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.5" style="1" customWidth="1"/>
-    <col min="35" max="35" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="10.875" style="1"/>
+    <col min="1" max="1" width="10.875" style="1"/>
+    <col min="2" max="2" width="13.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="1"/>
+    <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="17.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="7.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="37.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.5" style="1" customWidth="1"/>
+    <col min="36" max="36" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:41" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="7" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-      <c r="AE1" s="7"/>
-      <c r="AF1" s="7"/>
-      <c r="AG1" s="8" t="s">
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="8"/>
+      <c r="AE1" s="8"/>
+      <c r="AF1" s="8"/>
+      <c r="AG1" s="8"/>
+      <c r="AH1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="9" t="s">
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="AM1" s="9"/>
-      <c r="AN1" s="9"/>
+      <c r="AN1" s="10"/>
+      <c r="AO1" s="10"/>
     </row>
-    <row r="2" spans="1:40" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AI2" s="1" t="s">
+      <c r="AJ2" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AJ2" s="1" t="s">
+      <c r="AK2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AK2" s="1" t="s">
+      <c r="AL2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="AL2" s="1" t="s">
+      <c r="AM2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AM2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AN2" s="1" t="s">
+      <c r="AO2" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="63" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:41" ht="63" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="K3" s="1">
-        <v>1</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>1973</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>5297141</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="1">
         <v>50488261</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AA3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="AH3" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="AI3" s="1" t="s">
         <v>55</v>
       </c>
       <c r="AJ3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AK3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AK3" s="3" t="s">
+      <c r="AL3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AL3" s="1" t="s">
+      <c r="AM3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AM3" s="1" t="s">
+      <c r="AN3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AN3" s="1" t="s">
+      <c r="AO3" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:40" ht="63" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
+    <row r="4" spans="1:41" ht="63" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>1969</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="1">
+      <c r="T4" s="1">
         <v>4938795</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="V4" s="1">
+      <c r="W4" s="1">
         <v>47794774</v>
       </c>
-      <c r="W4" s="1" t="b">
+      <c r="X4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="W1:AF1"/>
-    <mergeCell ref="AG1:AK1"/>
-    <mergeCell ref="AL1:AN1"/>
-    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="X1:AG1"/>
+    <mergeCell ref="AH1:AL1"/>
+    <mergeCell ref="AM1:AO1"/>
+    <mergeCell ref="A1:W1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1403,25 +1412,25 @@
     </row>
     <row r="3" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -1460,238 +1469,241 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="21.625" customWidth="1"/>
-    <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="11" max="11" width="13.375" customWidth="1"/>
+    <col min="5" max="5" width="21.625" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="12" max="12" width="13.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
+      <c r="L1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="11" t="s">
+      <c r="M1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>71</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>7</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>8</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>72</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>46</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>57</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>43</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>40000000000002</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>30000000000004</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>74</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>1973</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>13</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>14</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>5297141</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>15</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>16</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>50488261</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>55</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>75</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>70</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>40000000000010</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>30000000000012</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
+      <c r="K3" s="1"/>
       <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>76</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>1969</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>29</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>30</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>4938795</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>31</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>32</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>47794774</v>
       </c>
-      <c r="W3" t="b">
+      <c r="X3" t="b">
         <v>1</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>77</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>78</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1708,231 +1720,234 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.625" customWidth="1"/>
-    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.875" customWidth="1"/>
-    <col min="26" max="26" width="17.375" customWidth="1"/>
+    <col min="5" max="6" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.625" customWidth="1"/>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="29.875" customWidth="1"/>
+    <col min="27" max="27" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
+      <c r="L1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="11" t="s">
+      <c r="M1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>71</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>7</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>8</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>72</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
         <v>85</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>40000000000002</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>30000000000004</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>74</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>1973</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>13</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>14</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>5297141</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>15</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>16</v>
       </c>
-      <c r="V2">
+      <c r="W2">
         <v>50488261</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>40000000000010</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>30000000000012</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
+      <c r="K3" s="1"/>
       <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>76</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <v>1969</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>29</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>30</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>4938795</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>31</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>32</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>47794774</v>
       </c>
-      <c r="W3" t="b">
+      <c r="X3" t="b">
         <v>1</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1949,295 +1964,298 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF3"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="5" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="17.125" customWidth="1"/>
-    <col min="13" max="13" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="37.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="26" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19" customWidth="1"/>
+    <col min="5" max="6" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="39.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="17.125" customWidth="1"/>
+    <col min="14" max="14" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
+      <c r="L1" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="11" t="s">
+      <c r="M1" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="K1" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="L1" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="1" t="s">
+    <row r="2" spans="1:33" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="4">
         <v>40000000000002</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="4">
         <v>30000000000004</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
-        <v>1</v>
-      </c>
+      <c r="K2" s="1"/>
       <c r="L2" s="1">
         <v>1</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="1">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="O2" s="1">
+      <c r="P2" s="1">
         <v>1973</v>
       </c>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="1">
+      <c r="T2" s="1">
         <v>5297141</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="V2" s="1">
+      <c r="W2" s="1">
         <v>50488261</v>
       </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="C3" s="1" t="s">
+    <row r="3" spans="1:33" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D3" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="4">
         <v>40000000000010</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="4">
         <v>30000000000012</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1">
-        <v>1</v>
-      </c>
+      <c r="K3" s="1"/>
       <c r="L3" s="1">
         <v>1</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1">
+      <c r="O3" s="1"/>
+      <c r="P3" s="1">
         <v>1969</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="1">
+      <c r="T3" s="1">
         <v>4938795</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="U3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="V3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="V3" s="1">
+      <c r="W3" s="1">
         <v>47794774</v>
       </c>
-      <c r="W3" s="1" t="b">
+      <c r="X3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
-      <c r="Z3" s="1" t="s">
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Added LP upload test, updated template, fixed display of conditional fields
</commit_message>
<xml_diff>
--- a/public/CSV_Import.xlsx
+++ b/public/CSV_Import.xlsx
@@ -14,9 +14,10 @@
   <sheets>
     <sheet name="Metadata fields for import" sheetId="1" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
-    <sheet name="sample dats" sheetId="3" r:id="rId3"/>
-    <sheet name="sample cdr" sheetId="4" r:id="rId4"/>
-    <sheet name="sample_open_reels" sheetId="5" r:id="rId5"/>
+    <sheet name="sample cdr" sheetId="4" r:id="rId3"/>
+    <sheet name="sample dats" sheetId="3" r:id="rId4"/>
+    <sheet name="sample_lps" sheetId="6" r:id="rId5"/>
+    <sheet name="sample_open_reels" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="146">
   <si>
     <t>Physical Object basic metadata fields</t>
   </si>
@@ -191,9 +192,6 @@
     <t>Catalog key</t>
   </si>
   <si>
-    <t>Has ephemira</t>
-  </si>
-  <si>
     <t>Pack deformation</t>
   </si>
   <si>
@@ -294,9 +292,6 @@
   </si>
   <si>
     <t>Other copies</t>
-  </si>
-  <si>
-    <t>Checkbox values in POD (Has Ephemira, Other Copies)</t>
   </si>
   <si>
     <t>True, TRUE, yes, X, x. Any text will evaluate to yes/true</t>
@@ -420,6 +415,138 @@
   </si>
   <si>
     <t>A blank or 0 value will not attempt to assign a Box or Bin.  Entering an MDPI Barcode value will attempt to use existing Bin/Box if found, or create a new one if not found.  Entering an invalid barcode, or one already assigned to a Physical Object, will produce an error.  Note creating a Bin via spreadsheet upload will generate a default Bin description.</t>
+  </si>
+  <si>
+    <t>Has ephemera</t>
+  </si>
+  <si>
+    <t>Diameter</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Groove size</t>
+  </si>
+  <si>
+    <t>Groove orientation</t>
+  </si>
+  <si>
+    <t>Recording method</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Substrate</t>
+  </si>
+  <si>
+    <t>Coating</t>
+  </si>
+  <si>
+    <t>Equalization</t>
+  </si>
+  <si>
+    <t>Country of origin</t>
+  </si>
+  <si>
+    <t>bin-id</t>
+  </si>
+  <si>
+    <t>LP</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>Delamination</t>
+  </si>
+  <si>
+    <t>Coarse</t>
+  </si>
+  <si>
+    <t>Lateral</t>
+  </si>
+  <si>
+    <t>Pressed</t>
+  </si>
+  <si>
+    <t>Shellac</t>
+  </si>
+  <si>
+    <t>RIAA</t>
+  </si>
+  <si>
+    <t>bin-id2</t>
+  </si>
+  <si>
+    <t>Scratched, Cracked</t>
+  </si>
+  <si>
+    <t>Exudation, Oxidation</t>
+  </si>
+  <si>
+    <t>Micro</t>
+  </si>
+  <si>
+    <t>Vertical</t>
+  </si>
+  <si>
+    <t>Cut</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Zinc</t>
+  </si>
+  <si>
+    <t>Lacquer</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>LP technical metadata fields</t>
+  </si>
+  <si>
+    <t>Broken, Cracked, Dirty, Fungus, Scratched, Warped, Worn</t>
+  </si>
+  <si>
+    <t>Delamination, Exudation, Oxidation</t>
+  </si>
+  <si>
+    <t>33.3 / 45 / 78</t>
+  </si>
+  <si>
+    <t>5 / 6 / 7 / 8 / 9 / 10 / 12 / 16</t>
+  </si>
+  <si>
+    <t>Coarse / Micro</t>
+  </si>
+  <si>
+    <t>Lateral / Vertical</t>
+  </si>
+  <si>
+    <t>Pressed / Cut / Pregrooved</t>
+  </si>
+  <si>
+    <t>Shellac / Plastic / N/A</t>
+  </si>
+  <si>
+    <t>Aluminum / Glass / Fiber / Steel / Zinc / N/A</t>
+  </si>
+  <si>
+    <t>None / Lacquer / N/A</t>
+  </si>
+  <si>
+    <t>RIAA / Other / Unknown</t>
+  </si>
+  <si>
+    <t>Copy</t>
+  </si>
+  <si>
+    <t>Checkbox values in POD (Has Ephemera, Other Copies)</t>
   </si>
 </sst>
 </file>
@@ -473,7 +600,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,6 +628,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,7 +687,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -585,6 +718,9 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -963,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO4"/>
+  <dimension ref="A1:BA4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1010,10 +1146,22 @@
     <col min="39" max="39" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="19.625" style="1" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="10.875" style="1"/>
+    <col min="42" max="42" width="13.625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="19.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.375" style="1" customWidth="1"/>
+    <col min="51" max="51" width="8.5" style="1" customWidth="1"/>
+    <col min="52" max="52" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:53" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1039,10 +1187,10 @@
       <c r="U1" s="11"/>
       <c r="V1" s="11"/>
       <c r="W1" s="11"/>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="11"/>
+      <c r="Y1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
       <c r="AA1" s="8"/>
       <c r="AB1" s="8"/>
@@ -1052,36 +1200,50 @@
       <c r="AF1" s="8"/>
       <c r="AG1" s="8"/>
       <c r="AH1" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AI1" s="9"/>
       <c r="AJ1" s="9"/>
       <c r="AK1" s="9"/>
       <c r="AL1" s="9"/>
       <c r="AM1" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AN1" s="10"/>
       <c r="AO1" s="10"/>
+      <c r="AP1" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="12"/>
+      <c r="AU1" s="12"/>
+      <c r="AV1" s="12"/>
+      <c r="AW1" s="12"/>
+      <c r="AX1" s="12"/>
+      <c r="AY1" s="12"/>
+      <c r="AZ1" s="12"/>
+      <c r="BA1" s="12"/>
     </row>
-    <row r="2" spans="1:41" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:53" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
@@ -1096,25 +1258,25 @@
         <v>42</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>43</v>
@@ -1132,69 +1294,105 @@
         <v>8</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AH2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI2" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="AJ2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AM2" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>111</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:41" ht="63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:53" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>115</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>10</v>
@@ -1212,10 +1410,10 @@
         <v>1</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P3" s="1">
         <v>1973</v>
@@ -1260,7 +1458,7 @@
         <v>23</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG3" s="1" t="s">
         <v>24</v>
@@ -1269,33 +1467,69 @@
         <v>25</v>
       </c>
       <c r="AI3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AJ3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AL3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AM3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="AN3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO3" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AO3" s="1" t="s">
-        <v>69</v>
+      <c r="AP3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:41" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:53" ht="63" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>144</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -1313,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P4" s="1">
         <v>1969</v>
@@ -1350,11 +1584,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="X1:AG1"/>
+  <mergeCells count="5">
     <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="AM1:AO1"/>
-    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="AP1:BA1"/>
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="Y1:AG1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1384,65 +1619,65 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>81</v>
+        <v>145</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
@@ -1469,35 +1704,57 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="21.625" customWidth="1"/>
-    <col min="6" max="6" width="32" customWidth="1"/>
-    <col min="12" max="12" width="13.375" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="42.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="99.75" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1512,25 +1769,25 @@
         <v>42</v>
       </c>
       <c r="K1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="N1" t="s">
         <v>4</v>
       </c>
       <c r="O1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P1" t="s">
         <v>5</v>
       </c>
       <c r="Q1" t="s">
-        <v>6</v>
+        <v>79</v>
       </c>
       <c r="R1" t="s">
         <v>43</v>
@@ -1548,27 +1805,24 @@
         <v>8</v>
       </c>
       <c r="W1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="X1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>66</v>
+        <v>102</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E2" s="4">
         <v>40000000000002</v>
@@ -1596,10 +1850,10 @@
         <v>1</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P2">
         <v>1973</v>
@@ -1622,22 +1876,19 @@
       <c r="W2">
         <v>50488261</v>
       </c>
-      <c r="Y2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>64</v>
+      <c r="Y2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E3" s="4">
         <v>40000000000010</v>
@@ -1665,10 +1916,10 @@
         <v>1</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P3">
         <v>1969</v>
@@ -1697,14 +1948,8 @@
       <c r="X3" t="b">
         <v>1</v>
       </c>
-      <c r="Y3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>78</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>79</v>
+      <c r="AA3" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1720,40 +1965,59 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="6" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.625" customWidth="1"/>
-    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="29.875" customWidth="1"/>
-    <col min="27" max="27" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="42.875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="99.75" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="42.875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
@@ -1768,25 +2032,25 @@
         <v>42</v>
       </c>
       <c r="K1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>95</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>97</v>
       </c>
       <c r="N1" t="s">
         <v>4</v>
       </c>
       <c r="O1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="P1" t="s">
         <v>5</v>
       </c>
       <c r="Q1" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="R1" t="s">
         <v>43</v>
@@ -1804,24 +2068,27 @@
         <v>8</v>
       </c>
       <c r="W1" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
         <v>72</v>
-      </c>
-      <c r="X1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
-        <v>85</v>
       </c>
       <c r="E2" s="4">
         <v>40000000000002</v>
@@ -1849,10 +2116,10 @@
         <v>1</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="P2">
         <v>1973</v>
@@ -1875,19 +2142,22 @@
       <c r="W2">
         <v>50488261</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="AA2" s="1" t="s">
+      <c r="Y2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA2" t="s">
         <v>69</v>
       </c>
+      <c r="AB2" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E3" s="4">
         <v>40000000000010</v>
@@ -1915,10 +2185,10 @@
         <v>1</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="P3">
         <v>1969</v>
@@ -1947,8 +2217,14 @@
       <c r="X3" t="b">
         <v>1</v>
       </c>
-      <c r="AA3" t="s">
-        <v>84</v>
+      <c r="Y3" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1963,6 +2239,338 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AG3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="42.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="99.75" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:33" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" t="s">
+        <v>7</v>
+      </c>
+      <c r="S1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" t="s">
+        <v>102</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>40000000000044</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="4">
+        <v>40000000000002</v>
+      </c>
+      <c r="F2" s="4">
+        <v>30000000000004</v>
+      </c>
+      <c r="G2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2">
+        <v>1973</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2">
+        <v>5297141</v>
+      </c>
+      <c r="R2" t="s">
+        <v>15</v>
+      </c>
+      <c r="S2" t="s">
+        <v>16</v>
+      </c>
+      <c r="T2">
+        <v>50488261</v>
+      </c>
+      <c r="W2" t="s">
+        <v>116</v>
+      </c>
+      <c r="X2">
+        <v>5</v>
+      </c>
+      <c r="Y2">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>40031234567896</v>
+      </c>
+      <c r="B3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E3" s="4">
+        <v>40000000000010</v>
+      </c>
+      <c r="F3" s="4">
+        <v>30000000000012</v>
+      </c>
+      <c r="G3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" t="s">
+        <v>75</v>
+      </c>
+      <c r="M3">
+        <v>1969</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3">
+        <v>4938795</v>
+      </c>
+      <c r="R3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3">
+        <v>47794774</v>
+      </c>
+      <c r="U3" t="b">
+        <v>1</v>
+      </c>
+      <c r="V3" t="s">
+        <v>123</v>
+      </c>
+      <c r="W3" t="s">
+        <v>124</v>
+      </c>
+      <c r="X3">
+        <v>16</v>
+      </c>
+      <c r="Y3">
+        <v>78</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>126</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>128</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>129</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>130</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG3"/>
   <sheetViews>
@@ -1996,110 +2604,110 @@
     <col min="32" max="32" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="L1" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E2" s="4">
         <v>40000000000002</v>
@@ -2127,10 +2735,10 @@
         <v>1</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P2" s="1">
         <v>1973</v>
@@ -2149,7 +2757,7 @@
         <v>15</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="W2" s="1">
         <v>50488261</v>
@@ -2177,7 +2785,7 @@
         <v>23</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG2" s="1" t="s">
         <v>24</v>
@@ -2185,7 +2793,7 @@
     </row>
     <row r="3" spans="1:33" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E3" s="4">
         <v>40000000000010</v>
@@ -2213,7 +2821,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
@@ -2235,7 +2843,7 @@
         <v>31</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="W3" s="1">
         <v>47794774</v>

</xml_diff>

<commit_message>
Added sound_field and label to interface, sound_field validation
</commit_message>
<xml_diff>
--- a/public/CSV_Import.xlsx
+++ b/public/CSV_Import.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7650" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7650" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata fields for import" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="149">
   <si>
     <t>Physical Object basic metadata fields</t>
   </si>
@@ -504,9 +504,6 @@
     <t>Lacquer</t>
   </si>
   <si>
-    <t>Canada</t>
-  </si>
-  <si>
     <t>LP technical metadata fields</t>
   </si>
   <si>
@@ -547,6 +544,18 @@
   </si>
   <si>
     <t>Checkbox values in POD (Has Ephemera, Other Copies)</t>
+  </si>
+  <si>
+    <t>Mono</t>
+  </si>
+  <si>
+    <t>Stereo</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Mono / Stereo / Unknown</t>
   </si>
 </sst>
 </file>
@@ -708,19 +717,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1099,9 +1108,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA4"/>
+  <dimension ref="A1:BC4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:X1"/>
     </sheetView>
   </sheetViews>
@@ -1156,12 +1165,14 @@
     <col min="49" max="49" width="7.75" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="11.375" style="1" customWidth="1"/>
     <col min="51" max="51" width="8.5" style="1" customWidth="1"/>
-    <col min="52" max="52" width="10.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="16384" width="10.875" style="1"/>
+    <col min="52" max="52" width="11.25" style="1" customWidth="1"/>
+    <col min="53" max="53" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.625" style="1" customWidth="1"/>
+    <col min="55" max="55" width="8.75" style="1" customWidth="1"/>
+    <col min="56" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1188,45 +1199,47 @@
       <c r="V1" s="11"/>
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="9" t="s">
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="10" t="s">
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="10"/>
+      <c r="AT1" s="10"/>
+      <c r="AU1" s="10"/>
+      <c r="AV1" s="10"/>
+      <c r="AW1" s="10"/>
+      <c r="AX1" s="10"/>
+      <c r="AY1" s="10"/>
+      <c r="AZ1" s="10"/>
+      <c r="BA1" s="10"/>
+      <c r="BB1" s="10"/>
+      <c r="BC1" s="10"/>
     </row>
-    <row r="2" spans="1:53" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>91</v>
       </c>
@@ -1381,13 +1394,19 @@
         <v>110</v>
       </c>
       <c r="AZ2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA2" t="s">
         <v>111</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>112</v>
       </c>
+      <c r="BC2" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="3" spans="1:53" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>88</v>
       </c>
@@ -1488,48 +1507,54 @@
         <v>68</v>
       </c>
       <c r="AP3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="AQ3" s="1" t="s">
+      <c r="AR3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AS3" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AS3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AT3" s="1" t="s">
+      <c r="AU3" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AV3" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AV3" s="1" t="s">
+      <c r="AW3" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AW3" s="1" t="s">
+      <c r="AX3" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AX3" s="1" t="s">
+      <c r="AY3" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="AY3" s="1" t="s">
+      <c r="AZ3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="BA3" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="AZ3" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="BA3" s="1" t="s">
+      <c r="BB3" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="BC3" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="4" spans="1:53" ht="63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" ht="63" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>88</v>
       </c>
       <c r="G4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>26</v>
@@ -1587,7 +1612,7 @@
   <mergeCells count="5">
     <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="AM1:AO1"/>
-    <mergeCell ref="AP1:BA1"/>
+    <mergeCell ref="AP1:BC1"/>
     <mergeCell ref="A1:X1"/>
     <mergeCell ref="Y1:AG1"/>
   </mergeCells>
@@ -1605,7 +1630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1671,7 +1696,7 @@
     </row>
     <row r="5" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>36</v>
@@ -2240,7 +2265,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AI3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2275,11 +2300,12 @@
     <col min="28" max="28" width="15.75" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="7.75" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.25" customWidth="1"/>
+    <col min="33" max="33" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>91</v>
       </c>
@@ -2374,13 +2400,19 @@
         <v>110</v>
       </c>
       <c r="AF1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>112</v>
       </c>
+      <c r="AI1" s="2" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>40000000000044</v>
       </c>
@@ -2463,13 +2495,19 @@
         <v>128</v>
       </c>
       <c r="AF2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AG2" t="s">
         <v>121</v>
       </c>
-      <c r="AG2" t="s">
-        <v>131</v>
+      <c r="AH2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>40031234567896</v>
       </c>
@@ -2561,6 +2599,9 @@
         <v>130</v>
       </c>
       <c r="AF3" t="s">
+        <v>146</v>
+      </c>
+      <c r="AG3" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated CSV_Import document, spec tests, and test upload file for Quantity handling.
</commit_message>
<xml_diff>
--- a/public/CSV_Import.xlsx
+++ b/public/CSV_Import.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aploshay\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7650" tabRatio="500"/>
+    <workbookView xWindow="1950" yWindow="720" windowWidth="15300" windowHeight="7650" tabRatio="735"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata fields for import" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="159">
   <si>
     <t>Physical Object basic metadata fields</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>Title</t>
-  </si>
-  <si>
-    <t>Orignal</t>
   </si>
   <si>
     <t>ohrc014</t>
@@ -163,9 +160,6 @@
       </rPr>
       <t xml:space="preserve"> text in the cell to denote that the metadata field should be set to yes/true. If the metadata field should be left unchecked in POD, leave the cell empty.</t>
     </r>
-  </si>
-  <si>
-    <t>Grouped metadata fields (Preservation Problems, Playback Speed, Sample Rate, etc)</t>
   </si>
   <si>
     <t>The spreadsheet should contain comma delimted values for those fields that should be set to yes/true in the POD</t>
@@ -557,6 +551,45 @@
   <si>
     <t>Mono / Stereo / Unknown</t>
   </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Conditions</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>First note; Additional note</t>
+  </si>
+  <si>
+    <t>Catalog Problem: Something is not right; Unplayable</t>
+  </si>
+  <si>
+    <t>Preservation Problems, Playback Speed, Sample Rate, etc.</t>
+  </si>
+  <si>
+    <t>Grouped metadata fields (sets of checkboxes)</t>
+  </si>
+  <si>
+    <t>Any text to import as one or more notes.  Notes are separated by semicolons, rather than commas, to allow use of commas in note text.</t>
+  </si>
+  <si>
+    <t>Normally left blank, you may enter a numeric value greater than 1 to created multiple records with the same information.  Note that if you specify an MDPI Barcode, only the first record will be created, as subsequent records will produce an error trying to re-use a unique MDPI barcode value.</t>
+  </si>
+  <si>
+    <t>You may specify one or more Condition Statuses to apply to the imported record.  You may optionally specify note text for the condition after a colon, in this format:
+&lt;condition name&gt;: &lt;note text&gt;
+You may specify multiple conditions by separating them with semicolons -- this allows use of commas in note text.
+Condition names must exactly match (with case-sensitivity) the list of Physical Object Condition Statuses specified in the POD.</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
 </sst>
 </file>
 
@@ -572,13 +605,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -608,8 +634,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,8 +680,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -655,48 +695,63 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -708,29 +763,35 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="38">
@@ -1108,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC4"/>
+  <dimension ref="A1:BF4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:X1"/>
+      <selection sqref="A1:AA1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1138,167 +1199,171 @@
     <col min="22" max="22" width="29.875" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.375" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5" style="1" customWidth="1"/>
-    <col min="36" max="36" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="12.5" style="1" customWidth="1"/>
+    <col min="28" max="28" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="37.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.5" style="1" customWidth="1"/>
+    <col min="39" max="39" width="15.125" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="19.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="10.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.375" style="1" customWidth="1"/>
-    <col min="51" max="51" width="8.5" style="1" customWidth="1"/>
-    <col min="52" max="52" width="11.25" style="1" customWidth="1"/>
-    <col min="53" max="53" width="10.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.625" style="1" customWidth="1"/>
-    <col min="55" max="55" width="8.75" style="1" customWidth="1"/>
-    <col min="56" max="16384" width="10.875" style="1"/>
+    <col min="41" max="41" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.625" style="1" customWidth="1"/>
+    <col min="46" max="46" width="19.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="5.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="15.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.375" style="1" customWidth="1"/>
+    <col min="54" max="54" width="8.5" style="1" customWidth="1"/>
+    <col min="55" max="55" width="11.25" style="1" customWidth="1"/>
+    <col min="56" max="56" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="14.625" style="1" customWidth="1"/>
+    <col min="58" max="58" width="8.75" style="1" customWidth="1"/>
+    <col min="59" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:58" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="12" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="8" t="s">
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
+      <c r="AP1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="AI1" s="8"/>
-      <c r="AJ1" s="8"/>
-      <c r="AK1" s="8"/>
-      <c r="AL1" s="8"/>
-      <c r="AM1" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AN1" s="9"/>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
-      <c r="AY1" s="10"/>
-      <c r="AZ1" s="10"/>
-      <c r="BA1" s="10"/>
-      <c r="BB1" s="10"/>
-      <c r="BC1" s="10"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
     </row>
-    <row r="2" spans="1:55" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="K2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>95</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>7</v>
@@ -1307,120 +1372,129 @@
         <v>8</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="X2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AR2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AV2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AW2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BB2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BC2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AH2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>107</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AX2" t="s">
+      <c r="BD2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="BE2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AZ2" t="s">
-        <v>52</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>111</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>112</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>147</v>
+      <c r="BF2" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:55" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="L3" s="1">
         <v>1</v>
@@ -1429,141 +1503,147 @@
         <v>1</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P3" s="1">
         <v>1973</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="T3" s="1">
         <v>5297141</v>
       </c>
       <c r="U3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="V3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="W3" s="1">
         <v>50488261</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Z3" s="1" t="s">
+      <c r="AD3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AE3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AF3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AG3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AD3" s="1" t="s">
+      <c r="AH3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AE3" s="1" t="s">
+      <c r="AI3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AF3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AK3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AH3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AI3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL3" s="3" t="s">
-        <v>63</v>
+      <c r="AL3" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="AN3" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="AO3" s="1" t="s">
-        <v>68</v>
+      <c r="AO3" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="AP3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AV3" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="AQ3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AW3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AX3" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="AS3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AT3" s="1" t="s">
+      <c r="AY3" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="AU3" s="1" t="s">
+      <c r="AZ3" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="AV3" s="1" t="s">
+      <c r="BA3" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="AW3" s="1" t="s">
+      <c r="BB3" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="AX3" s="1" t="s">
+      <c r="BC3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="BD3" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="AY3" s="1" t="s">
+      <c r="BE3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="BF3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" ht="63" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" t="s">
         <v>141</v>
       </c>
-      <c r="AZ3" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="BA3" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="BB3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BC3" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:55" ht="63" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" t="s">
-        <v>143</v>
-      </c>
       <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="L4" s="1">
         <v>1</v>
@@ -1572,28 +1652,28 @@
         <v>1</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P4" s="1">
         <v>1969</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="T4" s="1">
         <v>4938795</v>
       </c>
       <c r="U4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="W4" s="1">
         <v>47794774</v>
@@ -1601,20 +1681,20 @@
       <c r="X4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="AB4" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AM1:AO1"/>
-    <mergeCell ref="AP1:BC1"/>
-    <mergeCell ref="A1:X1"/>
-    <mergeCell ref="Y1:AG1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AR1"/>
+    <mergeCell ref="AS1:BF1"/>
+    <mergeCell ref="AB1:AJ1"/>
+    <mergeCell ref="A1:AA1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1628,7 +1708,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1643,77 +1723,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>61</v>
+      <c r="A1" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>86</v>
+      <c r="A2" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>90</v>
+      <c r="A4" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>144</v>
+      <c r="A5" s="5" t="s">
+        <v>142</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>21</v>
+      <c r="C9" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1729,7 +1860,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA3"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1757,71 +1888,72 @@
     <col min="22" max="22" width="99.75" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="12.625" customWidth="1"/>
+    <col min="28" max="28" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="N1" t="s">
         <v>4</v>
       </c>
       <c r="O1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P1" t="s">
         <v>5</v>
       </c>
       <c r="Q1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="R1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" t="s">
         <v>43</v>
-      </c>
-      <c r="S1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" t="s">
-        <v>45</v>
       </c>
       <c r="U1" t="s">
         <v>7</v>
@@ -1830,24 +1962,33 @@
         <v>8</v>
       </c>
       <c r="W1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="X1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>56</v>
+        <v>100</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" s="4">
         <v>40000000000002</v>
@@ -1856,16 +1997,16 @@
         <v>30000000000004</v>
       </c>
       <c r="G2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1">
@@ -1875,45 +2016,51 @@
         <v>1</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P2">
         <v>1973</v>
       </c>
       <c r="R2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" t="s">
         <v>13</v>
-      </c>
-      <c r="S2" t="s">
-        <v>14</v>
       </c>
       <c r="T2">
         <v>5297141</v>
       </c>
       <c r="U2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" t="s">
         <v>15</v>
-      </c>
-      <c r="V2" t="s">
-        <v>16</v>
       </c>
       <c r="W2">
         <v>50488261</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="Z2" s="1" t="s">
-        <v>67</v>
+        <v>150</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>68</v>
+        <v>151</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E3" s="4">
         <v>40000000000010</v>
@@ -1922,16 +2069,16 @@
         <v>30000000000012</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1">
@@ -1941,31 +2088,31 @@
         <v>1</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P3">
         <v>1969</v>
       </c>
       <c r="Q3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" t="s">
         <v>29</v>
-      </c>
-      <c r="S3" t="s">
-        <v>30</v>
       </c>
       <c r="T3">
         <v>4938795</v>
       </c>
       <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" t="s">
         <v>31</v>
-      </c>
-      <c r="V3" t="s">
-        <v>32</v>
       </c>
       <c r="W3">
         <v>47794774</v>
@@ -1973,8 +2120,8 @@
       <c r="X3" t="b">
         <v>1</v>
       </c>
-      <c r="AA3" t="s">
-        <v>82</v>
+      <c r="AD3" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1990,7 +2137,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2019,57 +2166,58 @@
     <col min="22" max="22" width="99.75" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="42.875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="12.625" customWidth="1"/>
+    <col min="28" max="28" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="42.875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="N1" t="s">
         <v>4</v>
       </c>
       <c r="O1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="P1" t="s">
         <v>5</v>
@@ -2078,13 +2226,13 @@
         <v>6</v>
       </c>
       <c r="R1" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" t="s">
         <v>43</v>
-      </c>
-      <c r="S1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" t="s">
-        <v>45</v>
       </c>
       <c r="U1" t="s">
         <v>7</v>
@@ -2093,27 +2241,36 @@
         <v>8</v>
       </c>
       <c r="W1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="X1" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>47</v>
+        <v>100</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>148</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>65</v>
+        <v>54</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E2" s="4">
         <v>40000000000002</v>
@@ -2122,16 +2279,16 @@
         <v>30000000000004</v>
       </c>
       <c r="G2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1">
@@ -2141,48 +2298,54 @@
         <v>1</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P2">
         <v>1973</v>
       </c>
       <c r="R2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" t="s">
         <v>13</v>
-      </c>
-      <c r="S2" t="s">
-        <v>14</v>
       </c>
       <c r="T2">
         <v>5297141</v>
       </c>
       <c r="U2" t="s">
+        <v>14</v>
+      </c>
+      <c r="V2" t="s">
         <v>15</v>
-      </c>
-      <c r="V2" t="s">
-        <v>16</v>
       </c>
       <c r="W2">
         <v>50488261</v>
       </c>
-      <c r="Y2" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>69</v>
+      <c r="Z2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="AB2" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E3" s="4">
         <v>40000000000010</v>
@@ -2191,16 +2354,16 @@
         <v>30000000000012</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
-      </c>
-      <c r="J3" t="s">
-        <v>28</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1">
@@ -2210,31 +2373,31 @@
         <v>1</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="P3">
         <v>1969</v>
       </c>
       <c r="Q3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R3" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" t="s">
         <v>29</v>
-      </c>
-      <c r="S3" t="s">
-        <v>30</v>
       </c>
       <c r="T3">
         <v>4938795</v>
       </c>
       <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" t="s">
         <v>31</v>
-      </c>
-      <c r="V3" t="s">
-        <v>32</v>
       </c>
       <c r="W3">
         <v>47794774</v>
@@ -2242,14 +2405,14 @@
       <c r="X3" t="b">
         <v>1</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="AB3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE3" t="s">
         <v>76</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2265,7 +2428,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI3"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2291,56 +2454,57 @@
     <col min="19" max="19" width="99.75" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.25" customWidth="1"/>
-    <col min="33" max="33" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="12.625" customWidth="1"/>
+    <col min="25" max="25" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.25" customWidth="1"/>
+    <col min="36" max="36" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
         <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
       </c>
       <c r="K1" t="s">
         <v>4</v>
       </c>
       <c r="L1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -2349,13 +2513,13 @@
         <v>6</v>
       </c>
       <c r="O1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
         <v>43</v>
-      </c>
-      <c r="P1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>45</v>
       </c>
       <c r="R1" t="s">
         <v>7</v>
@@ -2364,63 +2528,72 @@
         <v>8</v>
       </c>
       <c r="T1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="U1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="X1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="AF1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>147</v>
+      <c r="AL1" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>40000000000044</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E2" s="4">
         <v>40000000000002</v>
@@ -2429,93 +2602,99 @@
         <v>30000000000004</v>
       </c>
       <c r="G2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
-      <c r="J2" t="s">
-        <v>12</v>
-      </c>
       <c r="K2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M2">
         <v>1973</v>
       </c>
       <c r="O2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" t="s">
         <v>13</v>
-      </c>
-      <c r="P2" t="s">
-        <v>14</v>
       </c>
       <c r="Q2">
         <v>5297141</v>
       </c>
       <c r="R2" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" t="s">
         <v>15</v>
-      </c>
-      <c r="S2" t="s">
-        <v>16</v>
       </c>
       <c r="T2">
         <v>50488261</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AA2">
+        <v>5</v>
+      </c>
+      <c r="AB2">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AD2" t="s">
         <v>116</v>
       </c>
-      <c r="X2">
-        <v>5</v>
-      </c>
-      <c r="Y2">
-        <v>33.299999999999997</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AE2" t="s">
         <v>117</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AF2" t="s">
         <v>118</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AG2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>119</v>
       </c>
-      <c r="AC2" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>128</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>145</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>121</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>54</v>
+      <c r="AK2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>40031234567896</v>
       </c>
       <c r="B3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E3" s="4">
         <v>40000000000010</v>
@@ -2524,43 +2703,43 @@
         <v>30000000000012</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
-        <v>28</v>
-      </c>
       <c r="K3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M3">
         <v>1969</v>
       </c>
       <c r="N3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="P3" t="s">
         <v>29</v>
-      </c>
-      <c r="P3" t="s">
-        <v>30</v>
       </c>
       <c r="Q3">
         <v>4938795</v>
       </c>
       <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" t="s">
         <v>31</v>
-      </c>
-      <c r="S3" t="s">
-        <v>32</v>
       </c>
       <c r="T3">
         <v>47794774</v>
@@ -2568,41 +2747,41 @@
       <c r="U3" t="b">
         <v>1</v>
       </c>
-      <c r="V3" t="s">
+      <c r="Y3" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AA3">
+        <v>16</v>
+      </c>
+      <c r="AB3">
+        <v>78</v>
+      </c>
+      <c r="AC3" t="s">
         <v>123</v>
       </c>
-      <c r="W3" t="s">
+      <c r="AD3" t="s">
         <v>124</v>
       </c>
-      <c r="X3">
-        <v>16</v>
-      </c>
-      <c r="Y3">
-        <v>78</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="AE3" t="s">
         <v>125</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AF3" t="s">
         <v>126</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AG3" t="s">
         <v>127</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AH3" t="s">
         <v>128</v>
       </c>
-      <c r="AD3" t="s">
-        <v>129</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>130</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>82</v>
+      <c r="AI3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2613,7 +2792,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AJ3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2636,119 +2815,129 @@
     <col min="22" max="22" width="26.5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.375" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="26" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="12.5" customWidth="1"/>
+    <col min="28" max="28" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="26" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="17" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="L1" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" s="7" t="s">
+      <c r="M1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="S1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="R1" s="7" t="s">
+      <c r="T1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="U1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="V1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="AC1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>53</v>
-      </c>
     </row>
-    <row r="2" spans="1:33" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E2" s="4">
         <v>40000000000002</v>
@@ -2757,16 +2946,16 @@
         <v>30000000000004</v>
       </c>
       <c r="G2" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="1">
@@ -2776,65 +2965,72 @@
         <v>1</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="P2" s="1">
         <v>1973</v>
       </c>
       <c r="Q2" s="1"/>
       <c r="R2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="T2" s="1">
         <v>5297141</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="W2" s="1">
         <v>50488261</v>
       </c>
       <c r="X2" s="1"/>
-      <c r="Y2" s="1" t="s">
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AF2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="3" spans="1:33" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="31.5" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E3" s="4">
         <v>40000000000010</v>
@@ -2843,16 +3039,16 @@
         <v>30000000000012</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>113</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1">
@@ -2862,29 +3058,29 @@
         <v>1</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O3" s="1"/>
       <c r="P3" s="1">
         <v>1969</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="R3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="T3" s="1">
         <v>4938795</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="W3" s="1">
         <v>47794774</v>
@@ -2894,17 +3090,20 @@
       </c>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>
-      <c r="AA3" s="1" t="s">
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC3" s="1"/>
-      <c r="AD3" s="1"/>
-      <c r="AE3" s="1"/>
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Spreadsheet import: deprecated Quantity, changed Notes/Conditions delimiter to pipe(s), forked Internal Notes and External notes (export=true).
</commit_message>
<xml_diff>
--- a/public/CSV_Import.xlsx
+++ b/public/CSV_Import.xlsx
@@ -5,11 +5,11 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="720" windowWidth="15300" windowHeight="7650" tabRatio="735"/>
+    <workbookView xWindow="2925" yWindow="1080" windowWidth="15300" windowHeight="7650" tabRatio="735"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata fields for import" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="163">
   <si>
     <t>Physical Object basic metadata fields</t>
   </si>
@@ -552,18 +552,12 @@
     <t>Mono / Stereo / Unknown</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Conditions</t>
   </si>
   <si>
     <t>Quantity</t>
   </si>
   <si>
-    <t>First note; Additional note</t>
-  </si>
-  <si>
     <t>Catalog Problem: Something is not right; Unplayable</t>
   </si>
   <si>
@@ -571,12 +565,6 @@
   </si>
   <si>
     <t>Grouped metadata fields (sets of checkboxes)</t>
-  </si>
-  <si>
-    <t>Any text to import as one or more notes.  Notes are separated by semicolons, rather than commas, to allow use of commas in note text.</t>
-  </si>
-  <si>
-    <t>Normally left blank, you may enter a numeric value greater than 1 to created multiple records with the same information.  Note that if you specify an MDPI Barcode, only the first record will be created, as subsequent records will produce an error trying to re-use a unique MDPI barcode value.</t>
   </si>
   <si>
     <t>You may specify one or more Condition Statuses to apply to the imported record.  You may optionally specify note text for the condition after a colon, in this format:
@@ -589,6 +577,31 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Internal Notes</t>
+  </si>
+  <si>
+    <t>External Notes</t>
+  </si>
+  <si>
+    <t>First note | Additional note</t>
+  </si>
+  <si>
+    <t>Note 1 | Note 2</t>
+  </si>
+  <si>
+    <t>Catalog Problem: Something is not right| Unplayable</t>
+  </si>
+  <si>
+    <t>Internal/External Notes</t>
+  </si>
+  <si>
+    <t>Internal Notes, External Notes</t>
+  </si>
+  <si>
+    <t>Any text to import as one or more notes.  Notes are separated by the "pipe" character, | (shift + \).
+External Notes are imported with the checkbox for shipping manifest report inclusion checked; Internal Notes are not.</t>
   </si>
 </sst>
 </file>
@@ -751,7 +764,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -769,20 +782,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -791,6 +795,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1235,74 +1245,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:58" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="11" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="12" t="s">
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="13" t="s">
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="14" t="s">
+      <c r="AQ1" s="10"/>
+      <c r="AR1" s="10"/>
+      <c r="AS1" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="14"/>
-      <c r="AV1" s="14"/>
-      <c r="AW1" s="14"/>
-      <c r="AX1" s="14"/>
-      <c r="AY1" s="14"/>
-      <c r="AZ1" s="14"/>
-      <c r="BA1" s="14"/>
-      <c r="BB1" s="14"/>
-      <c r="BC1" s="14"/>
-      <c r="BD1" s="14"/>
-      <c r="BE1" s="14"/>
-      <c r="BF1" s="14"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11"/>
     </row>
     <row r="2" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1378,13 +1388,13 @@
         <v>100</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="Z2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>44</v>
@@ -1529,11 +1539,14 @@
       <c r="W3" s="1">
         <v>50488261</v>
       </c>
+      <c r="Y3" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="Z3" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>16</v>
@@ -1708,7 +1721,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1723,19 +1736,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="A1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1791,59 +1804,45 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="126" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="7">
-        <v>3</v>
+        <v>162</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>157</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>147</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>147</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="D8" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1860,7 +1859,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1888,13 +1887,13 @@
     <col min="22" max="22" width="99.75" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="12.625" customWidth="1"/>
-    <col min="28" max="28" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="12.625" customWidth="1"/>
+    <col min="29" max="29" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>89</v>
       </c>
@@ -1968,25 +1967,28 @@
         <v>100</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="Z1" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="AA1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB1" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="AA1" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:30" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>81</v>
       </c>
@@ -2043,22 +2045,25 @@
         <v>50488261</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="AB2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>81</v>
       </c>
@@ -2120,7 +2125,7 @@
       <c r="X3" t="b">
         <v>1</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2247,13 +2252,13 @@
         <v>100</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="Z1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>54</v>
@@ -2324,11 +2329,14 @@
       <c r="W2">
         <v>50488261</v>
       </c>
+      <c r="Y2" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="Z2" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="AB2" t="s">
         <v>52</v>
@@ -2534,13 +2542,13 @@
         <v>100</v>
       </c>
       <c r="V1" s="6" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="W1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="X1" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="X1" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>34</v>
@@ -2640,11 +2648,14 @@
       <c r="T2">
         <v>50488261</v>
       </c>
+      <c r="V2" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="W2" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="Z2" t="s">
         <v>114</v>
@@ -2899,13 +2910,13 @@
         <v>100</v>
       </c>
       <c r="Y1" s="6" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="Z1" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="AA1" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>44</v>
@@ -2993,12 +3004,14 @@
         <v>50488261</v>
       </c>
       <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
+      <c r="Y2" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="Z2" s="1" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
[POD-1471] Updated spreadsheet upload template .xlsx
</commit_message>
<xml_diff>
--- a/public/CSV_Import.xlsx
+++ b/public/CSV_Import.xlsx
@@ -5,19 +5,20 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aploshay\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="2925" yWindow="1080" windowWidth="15300" windowHeight="7650" tabRatio="735"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata fields for import" sheetId="1" r:id="rId1"/>
+    <sheet name="Minimal fields for import" sheetId="7" r:id="rId1"/>
     <sheet name="Notes" sheetId="2" r:id="rId2"/>
-    <sheet name="sample cdr" sheetId="4" r:id="rId3"/>
-    <sheet name="sample dats" sheetId="3" r:id="rId4"/>
-    <sheet name="sample_lps" sheetId="6" r:id="rId5"/>
-    <sheet name="sample_open_reels" sheetId="5" r:id="rId6"/>
+    <sheet name="Metadata fields for import" sheetId="1" r:id="rId3"/>
+    <sheet name="sample cdr" sheetId="4" r:id="rId4"/>
+    <sheet name="sample dats" sheetId="3" r:id="rId5"/>
+    <sheet name="sample_lps" sheetId="6" r:id="rId6"/>
+    <sheet name="sample_open_reels" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="180">
   <si>
     <t>Physical Object basic metadata fields</t>
   </si>
@@ -603,12 +604,63 @@
     <t>Any text to import as one or more notes.  Notes are separated by the "pipe" character, | (shift + \).
 External Notes are imported with the checkbox for shipping manifest report inclusion checked; Internal Notes are not.</t>
   </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Example:</t>
+  </si>
+  <si>
+    <t>At least one of these 4 fields must be provided.  If MDPI barcode is provided, it must be a valid barcode not already in use by any existing physical object, box, or bin.</t>
+  </si>
+  <si>
+    <t>Some stand-alone work</t>
+  </si>
+  <si>
+    <t>Another stand-alone work</t>
+  </si>
+  <si>
+    <t>For a multi-volume work:</t>
+  </si>
+  <si>
+    <t>For a stand-alone work:</t>
+  </si>
+  <si>
+    <t>(leave blank)</t>
+  </si>
+  <si>
+    <t>The volume number -- 1for the first, etc.</t>
+  </si>
+  <si>
+    <t>If there are any multi-volume works, they must be listed sequentially, and grouping information must also be provided:</t>
+  </si>
+  <si>
+    <t>Some value (unique within this column of the spreadsheet) that identifies these volumes as belonging to the same work.  Ex. "The Lord of the Rings Trilogy"</t>
+  </si>
+  <si>
+    <t>The Lord of the Rings Trilogy</t>
+  </si>
+  <si>
+    <t>The Fellowship of the Ring</t>
+  </si>
+  <si>
+    <t>The Two Towers</t>
+  </si>
+  <si>
+    <t>The Return of the King</t>
+  </si>
+  <si>
+    <t>Total volumes in the work, as published, even if you are missing volumes -- usually equivalent to the last group position you a providing, unless you are missing any volumes.</t>
+  </si>
+  <si>
+    <t>Minimum fields for basic import are:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -655,8 +707,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -699,8 +759,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -721,6 +811,92 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -764,7 +940,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -802,6 +978,65 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="38">
@@ -1179,10 +1414,478 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BF4"/>
+  <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AA1"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36" style="1" customWidth="1"/>
+    <col min="3" max="3" width="30.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.75" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="32.375" customWidth="1"/>
+    <col min="7" max="7" width="25" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="17.125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="13.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="12.5" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="31"/>
+    </row>
+    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="31"/>
+    </row>
+    <row r="7" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="32"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C10" s="33">
+        <v>40000000001234</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="34">
+        <v>40000000001235</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="63" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="29" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="G20" s="23"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="23"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H21" s="26">
+        <v>1</v>
+      </c>
+      <c r="I21" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="H22" s="28">
+        <v>2</v>
+      </c>
+      <c r="I22" s="28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="14">
+        <v>3</v>
+      </c>
+      <c r="I23" s="14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B4:B7"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BE4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1202,49 +1905,48 @@
     <col min="15" max="15" width="13.125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="24" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="12.5" style="1" customWidth="1"/>
-    <col min="28" max="28" width="15.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="8.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="37.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="17.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.5" style="1" customWidth="1"/>
-    <col min="39" max="39" width="15.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.625" style="1" customWidth="1"/>
-    <col min="46" max="46" width="19.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="5.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="10.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="16.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.375" style="1" customWidth="1"/>
-    <col min="54" max="54" width="8.5" style="1" customWidth="1"/>
-    <col min="55" max="55" width="11.25" style="1" customWidth="1"/>
-    <col min="56" max="56" width="10.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="14.625" style="1" customWidth="1"/>
-    <col min="58" max="58" width="8.75" style="1" customWidth="1"/>
-    <col min="59" max="16384" width="10.875" style="1"/>
+    <col min="18" max="18" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="26" width="12.5" style="1" customWidth="1"/>
+    <col min="27" max="27" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="37.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="17.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.5" style="1" customWidth="1"/>
+    <col min="38" max="38" width="15.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.625" style="1" customWidth="1"/>
+    <col min="45" max="45" width="19.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="5.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="10.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="15.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="11.375" style="1" customWidth="1"/>
+    <col min="53" max="53" width="8.5" style="1" customWidth="1"/>
+    <col min="54" max="54" width="11.25" style="1" customWidth="1"/>
+    <col min="55" max="55" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.625" style="1" customWidth="1"/>
+    <col min="57" max="57" width="8.75" style="1" customWidth="1"/>
+    <col min="58" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1273,10 +1975,10 @@
       <c r="X1" s="13"/>
       <c r="Y1" s="13"/>
       <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="12" t="s">
+      <c r="AA1" s="12" t="s">
         <v>1</v>
       </c>
+      <c r="AB1" s="12"/>
       <c r="AC1" s="12"/>
       <c r="AD1" s="12"/>
       <c r="AE1" s="12"/>
@@ -1284,22 +1986,22 @@
       <c r="AG1" s="12"/>
       <c r="AH1" s="12"/>
       <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="9" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>62</v>
       </c>
+      <c r="AK1" s="9"/>
       <c r="AL1" s="9"/>
       <c r="AM1" s="9"/>
       <c r="AN1" s="9"/>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="10" t="s">
+      <c r="AO1" s="10" t="s">
         <v>64</v>
       </c>
+      <c r="AP1" s="10"/>
       <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="11" t="s">
+      <c r="AR1" s="11" t="s">
         <v>129</v>
       </c>
+      <c r="AS1" s="11"/>
       <c r="AT1" s="11"/>
       <c r="AU1" s="11"/>
       <c r="AV1" s="11"/>
@@ -1312,9 +2014,8 @@
       <c r="BC1" s="11"/>
       <c r="BD1" s="11"/>
       <c r="BE1" s="11"/>
-      <c r="BF1" s="11"/>
-    </row>
-    <row r="2" spans="1:58" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:57" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>89</v>
       </c>
@@ -1367,130 +2068,127 @@
         <v>77</v>
       </c>
       <c r="R2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AI2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AE2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AH2" s="1" t="s">
+      <c r="AN2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AP2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AR2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AT2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AV2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AX2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AY2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="BB2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AI2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AJ2" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="AL2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO2" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="AP2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AQ2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AR2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AT2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU2" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="AW2" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="AX2" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AY2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AZ2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="BA2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="BB2" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="BC2" s="2" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="BD2" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="BF2" s="2" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:58" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" ht="78.75" x14ac:dyDescent="0.25">
       <c r="D3" s="1" t="s">
         <v>86</v>
       </c>
@@ -1522,127 +2220,124 @@
         <v>1973</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T3" s="1">
+      <c r="S3" s="1">
         <v>5297141</v>
       </c>
+      <c r="T3" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="U3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="W3" s="1">
+      <c r="V3" s="1">
         <v>50488261</v>
       </c>
+      <c r="X3" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="Y3" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>159</v>
+        <v>16</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="AI3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK3" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="AJ3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK3" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="AL3" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AM3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AP3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR3" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS3" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AT3" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AV3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AW3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AX3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AY3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ3" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BA3" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="BB3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="BC3" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="BD3" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="AN3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="AO3" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="AP3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="AR3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS3" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AT3" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AU3" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AV3" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AW3" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AX3" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AY3" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AZ3" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="BA3" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="BB3" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="BC3" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="BD3" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="BE3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="BF3" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:58" ht="63" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:57" ht="63" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>86</v>
       </c>
@@ -1674,40 +2369,37 @@
         <v>37</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="1">
+      <c r="S4" s="1">
         <v>4938795</v>
       </c>
+      <c r="T4" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="U4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="W4" s="1">
+      <c r="V4" s="1">
         <v>47794774</v>
       </c>
-      <c r="X4" s="1" t="b">
+      <c r="W4" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="AC4" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="AD4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE4" s="1" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AR1"/>
-    <mergeCell ref="AS1:BF1"/>
-    <mergeCell ref="AB1:AJ1"/>
-    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AQ1"/>
+    <mergeCell ref="AR1:BE1"/>
+    <mergeCell ref="AA1:AI1"/>
+    <mergeCell ref="A1:Z1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1719,145 +2411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="43.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE3"/>
   <sheetViews>
@@ -2140,7 +2694,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE3"/>
   <sheetViews>
@@ -2434,7 +2988,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL3"/>
   <sheetViews>
@@ -2801,7 +3355,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ3"/>
   <sheetViews>

</xml_diff>